<commit_message>
added missing data (heval 1, heval 2)
</commit_message>
<xml_diff>
--- a/data/processed/MASTER_human-eval.xlsx
+++ b/data/processed/MASTER_human-eval.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="206">
   <si>
     <t xml:space="preserve">source</t>
   </si>
@@ -317,6 +317,12 @@
     <t xml:space="preserve">newspaper_ampel-aus_300-400_processed.json_89</t>
   </si>
   <si>
+    <t xml:space="preserve">170</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newspaper_ampel-aus_0-200_processed.json_170</t>
+  </si>
+  <si>
     <t xml:space="preserve">Henri</t>
   </si>
   <si>
@@ -459,6 +465,36 @@
   </si>
   <si>
     <t xml:space="preserve">newspaper_ampel-aus_0-200_processed.json_137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newspaper_ampel-aus_0-200_processed.json_152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">169</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not realy about the coallition breakdown </t>
+  </si>
+  <si>
+    <t xml:space="preserve">newspaper_ampel-aus_0-200_processed.json_169</t>
+  </si>
+  <si>
+    <t xml:space="preserve">177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newspaper_ampel-aus_0-200_processed.json_177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">197</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newspaper_ampel-aus_0-200_processed.json_197</t>
   </si>
   <si>
     <t xml:space="preserve">200</t>
@@ -3015,13 +3051,13 @@
         <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C34" t="s">
         <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E34" t="s">
         <v>25</v>
@@ -3048,29 +3084,29 @@
         <v>26</v>
       </c>
       <c r="M34" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N34" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="O34" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="P34" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="Q34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="T34"/>
       <c r="U34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35">
@@ -3078,10 +3114,10 @@
         <v>21</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C35" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="D35" t="s">
         <v>104</v>
@@ -3096,40 +3132,40 @@
         <v>27</v>
       </c>
       <c r="H35" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I35" t="s">
         <v>27</v>
       </c>
       <c r="J35" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K35" t="s">
         <v>26</v>
       </c>
       <c r="L35" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T35"/>
       <c r="U35" t="s">
@@ -3141,16 +3177,16 @@
         <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C36" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="D36" t="s">
         <v>106</v>
       </c>
       <c r="E36" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F36" t="s">
         <v>26</v>
@@ -3165,31 +3201,31 @@
         <v>27</v>
       </c>
       <c r="J36" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K36" t="s">
         <v>26</v>
       </c>
       <c r="L36" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M36" t="s">
         <v>27</v>
       </c>
       <c r="N36" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O36" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P36" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q36" t="s">
         <v>28</v>
       </c>
       <c r="R36" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S36" t="s">
         <v>28</v>
@@ -3204,16 +3240,16 @@
         <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D37" t="s">
         <v>108</v>
       </c>
       <c r="E37" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F37" t="s">
         <v>26</v>
@@ -3225,34 +3261,34 @@
         <v>26</v>
       </c>
       <c r="I37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K37" t="s">
         <v>26</v>
       </c>
       <c r="L37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M37" t="s">
         <v>27</v>
       </c>
       <c r="N37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P37" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Q37" t="s">
         <v>28</v>
       </c>
       <c r="R37" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S37" t="s">
         <v>28</v>
@@ -3267,19 +3303,19 @@
         <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C38" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="D38" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="E38" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F38" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G38" t="s">
         <v>27</v>
@@ -3291,7 +3327,7 @@
         <v>28</v>
       </c>
       <c r="J38" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K38" t="s">
         <v>26</v>
@@ -3303,7 +3339,7 @@
         <v>27</v>
       </c>
       <c r="N38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O38" t="s">
         <v>26</v>
@@ -3312,7 +3348,7 @@
         <v>28</v>
       </c>
       <c r="Q38" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="R38" t="s">
         <v>26</v>
@@ -3322,7 +3358,7 @@
       </c>
       <c r="T38"/>
       <c r="U38" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39">
@@ -3330,62 +3366,62 @@
         <v>21</v>
       </c>
       <c r="B39" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C39" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D39" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="E39" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F39" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H39" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I39" t="s">
         <v>28</v>
       </c>
       <c r="J39" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K39" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L39" t="s">
         <v>28</v>
       </c>
       <c r="M39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N39" t="s">
         <v>28</v>
       </c>
       <c r="O39" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P39" t="s">
         <v>28</v>
       </c>
       <c r="Q39" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="R39" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="S39" t="s">
         <v>28</v>
       </c>
       <c r="T39"/>
       <c r="U39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40">
@@ -3393,28 +3429,28 @@
         <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C40" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D40" t="s">
         <v>114</v>
       </c>
       <c r="E40" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H40" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J40" t="s">
         <v>28</v>
@@ -3426,16 +3462,16 @@
         <v>28</v>
       </c>
       <c r="M40" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N40" t="s">
         <v>28</v>
       </c>
       <c r="O40" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="P40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q40" t="s">
         <v>28</v>
@@ -3456,62 +3492,62 @@
         <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C41" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="D41" t="s">
-        <v>35</v>
+        <v>116</v>
       </c>
       <c r="E41" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J41" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K41" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L41" t="s">
         <v>28</v>
       </c>
       <c r="M41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N41" t="s">
         <v>28</v>
       </c>
       <c r="O41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q41" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R41" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S41" t="s">
         <v>28</v>
       </c>
       <c r="T41"/>
       <c r="U41" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42">
@@ -3519,13 +3555,13 @@
         <v>21</v>
       </c>
       <c r="B42" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C42" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D42" t="s">
-        <v>117</v>
+        <v>35</v>
       </c>
       <c r="E42" t="s">
         <v>25</v>
@@ -3537,13 +3573,13 @@
         <v>28</v>
       </c>
       <c r="H42" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I42" t="s">
         <v>28</v>
       </c>
       <c r="J42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K42" t="s">
         <v>27</v>
@@ -3564,7 +3600,7 @@
         <v>28</v>
       </c>
       <c r="Q42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R42" t="s">
         <v>27</v>
@@ -3582,7 +3618,7 @@
         <v>21</v>
       </c>
       <c r="B43" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C43" t="s">
         <v>23</v>
@@ -3600,7 +3636,7 @@
         <v>28</v>
       </c>
       <c r="H43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I43" t="s">
         <v>28</v>
@@ -3642,46 +3678,46 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" t="s">
         <v>121</v>
       </c>
-      <c r="B44" t="s">
-        <v>22</v>
-      </c>
-      <c r="C44" t="s">
-        <v>30</v>
-      </c>
-      <c r="D44" t="s">
-        <v>122</v>
-      </c>
       <c r="E44" t="s">
         <v>25</v>
       </c>
       <c r="F44" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G44" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H44" t="s">
         <v>27</v>
       </c>
       <c r="I44" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J44" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K44" t="s">
         <v>27</v>
       </c>
       <c r="L44" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M44" t="s">
         <v>27</v>
       </c>
       <c r="N44" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O44" t="s">
         <v>27</v>
@@ -3690,7 +3726,7 @@
         <v>28</v>
       </c>
       <c r="Q44" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R44" t="s">
         <v>27</v>
@@ -3700,12 +3736,12 @@
       </c>
       <c r="T44"/>
       <c r="U44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B45" t="s">
         <v>22</v>
@@ -3732,10 +3768,10 @@
         <v>27</v>
       </c>
       <c r="J45" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K45" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L45" t="s">
         <v>27</v>
@@ -3744,22 +3780,22 @@
         <v>27</v>
       </c>
       <c r="N45" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O45" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P45" t="s">
         <v>28</v>
       </c>
       <c r="Q45" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R45" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S45" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="T45"/>
       <c r="U45" t="s">
@@ -3768,7 +3804,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B46" t="s">
         <v>22</v>
@@ -3786,43 +3822,43 @@
         <v>26</v>
       </c>
       <c r="G46" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H46" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M46" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N46" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="O46" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="P46" t="s">
         <v>28</v>
       </c>
       <c r="Q46" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R46" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="S46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T46"/>
       <c r="U46" t="s">
@@ -3831,7 +3867,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B47" t="s">
         <v>22</v>
@@ -3840,7 +3876,7 @@
         <v>30</v>
       </c>
       <c r="D47" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="E47" t="s">
         <v>25</v>
@@ -3849,28 +3885,28 @@
         <v>26</v>
       </c>
       <c r="G47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H47" t="s">
         <v>26</v>
       </c>
       <c r="I47" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J47" t="s">
         <v>27</v>
       </c>
       <c r="K47" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L47" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M47" t="s">
         <v>26</v>
       </c>
       <c r="N47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O47" t="s">
         <v>26</v>
@@ -3889,12 +3925,12 @@
       </c>
       <c r="T47"/>
       <c r="U47" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B48" t="s">
         <v>22</v>
@@ -3903,49 +3939,49 @@
         <v>30</v>
       </c>
       <c r="D48" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="E48" t="s">
         <v>25</v>
       </c>
       <c r="F48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G48" t="s">
         <v>27</v>
       </c>
       <c r="H48" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K48" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N48" t="s">
         <v>27</v>
       </c>
       <c r="O48" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P48" t="s">
         <v>28</v>
       </c>
       <c r="Q48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R48" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="S48" t="s">
         <v>28</v>
@@ -3957,10 +3993,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B49" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C49" t="s">
         <v>30</v>
@@ -3969,7 +4005,7 @@
         <v>131</v>
       </c>
       <c r="E49" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F49" t="s">
         <v>27</v>
@@ -3978,19 +4014,19 @@
         <v>27</v>
       </c>
       <c r="H49" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I49" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J49" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="K49" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L49" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M49" t="s">
         <v>27</v>
@@ -3999,16 +4035,16 @@
         <v>27</v>
       </c>
       <c r="O49" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P49" t="s">
         <v>28</v>
       </c>
       <c r="Q49" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="R49" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S49" t="s">
         <v>28</v>
@@ -4020,7 +4056,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B50" t="s">
         <v>40</v>
@@ -4035,57 +4071,55 @@
         <v>27</v>
       </c>
       <c r="F50" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J50" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K50" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M50" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P50" t="s">
         <v>28</v>
       </c>
       <c r="Q50" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="R50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S50" t="s">
         <v>28</v>
       </c>
-      <c r="T50" t="s">
+      <c r="T50"/>
+      <c r="U50" t="s">
         <v>134</v>
-      </c>
-      <c r="U50" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B51" t="s">
         <v>40</v>
@@ -4094,61 +4128,63 @@
         <v>30</v>
       </c>
       <c r="D51" t="s">
+        <v>135</v>
+      </c>
+      <c r="E51" t="s">
+        <v>27</v>
+      </c>
+      <c r="F51" t="s">
+        <v>26</v>
+      </c>
+      <c r="G51" t="s">
+        <v>28</v>
+      </c>
+      <c r="H51" t="s">
+        <v>28</v>
+      </c>
+      <c r="I51" t="s">
+        <v>28</v>
+      </c>
+      <c r="J51" t="s">
+        <v>28</v>
+      </c>
+      <c r="K51" t="s">
+        <v>28</v>
+      </c>
+      <c r="L51" t="s">
+        <v>28</v>
+      </c>
+      <c r="M51" t="s">
+        <v>26</v>
+      </c>
+      <c r="N51" t="s">
+        <v>28</v>
+      </c>
+      <c r="O51" t="s">
+        <v>28</v>
+      </c>
+      <c r="P51" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>28</v>
+      </c>
+      <c r="R51" t="s">
+        <v>28</v>
+      </c>
+      <c r="S51" t="s">
+        <v>28</v>
+      </c>
+      <c r="T51" t="s">
         <v>136</v>
       </c>
-      <c r="E51" t="s">
-        <v>25</v>
-      </c>
-      <c r="F51" t="s">
-        <v>27</v>
-      </c>
-      <c r="G51" t="s">
-        <v>28</v>
-      </c>
-      <c r="H51" t="s">
-        <v>28</v>
-      </c>
-      <c r="I51" t="s">
-        <v>25</v>
-      </c>
-      <c r="J51" t="s">
-        <v>28</v>
-      </c>
-      <c r="K51" t="s">
-        <v>26</v>
-      </c>
-      <c r="L51" t="s">
-        <v>28</v>
-      </c>
-      <c r="M51" t="s">
-        <v>27</v>
-      </c>
-      <c r="N51" t="s">
-        <v>28</v>
-      </c>
-      <c r="O51" t="s">
-        <v>28</v>
-      </c>
-      <c r="P51" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q51" t="s">
-        <v>28</v>
-      </c>
-      <c r="R51" t="s">
-        <v>26</v>
-      </c>
-      <c r="S51" t="s">
-        <v>28</v>
-      </c>
-      <c r="T51"/>
       <c r="U51" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B52" t="s">
         <v>40</v>
@@ -4160,25 +4196,25 @@
         <v>138</v>
       </c>
       <c r="E52" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F52" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G52" t="s">
         <v>28</v>
       </c>
       <c r="H52" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I52" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J52" t="s">
         <v>28</v>
       </c>
       <c r="K52" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L52" t="s">
         <v>28</v>
@@ -4190,16 +4226,16 @@
         <v>28</v>
       </c>
       <c r="O52" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="P52" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="Q52" t="s">
         <v>28</v>
       </c>
       <c r="R52" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="S52" t="s">
         <v>28</v>
@@ -4211,10 +4247,10 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B53" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C53" t="s">
         <v>30</v>
@@ -4223,10 +4259,10 @@
         <v>140</v>
       </c>
       <c r="E53" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F53" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G53" t="s">
         <v>28</v>
@@ -4235,13 +4271,13 @@
         <v>26</v>
       </c>
       <c r="I53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J53" t="s">
         <v>28</v>
       </c>
       <c r="K53" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L53" t="s">
         <v>28</v>
@@ -4253,7 +4289,7 @@
         <v>28</v>
       </c>
       <c r="O53" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P53" t="s">
         <v>28</v>
@@ -4262,7 +4298,7 @@
         <v>28</v>
       </c>
       <c r="R53" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="S53" t="s">
         <v>28</v>
@@ -4274,7 +4310,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B54" t="s">
         <v>49</v>
@@ -4289,43 +4325,43 @@
         <v>25</v>
       </c>
       <c r="F54" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G54" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H54" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I54" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J54" t="s">
         <v>28</v>
       </c>
       <c r="K54" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L54" t="s">
         <v>28</v>
       </c>
       <c r="M54" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N54" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O54" t="s">
         <v>27</v>
       </c>
       <c r="P54" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q54" t="s">
         <v>28</v>
       </c>
       <c r="R54" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="S54" t="s">
         <v>28</v>
@@ -4337,7 +4373,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B55" t="s">
         <v>49</v>
@@ -4346,40 +4382,40 @@
         <v>30</v>
       </c>
       <c r="D55" t="s">
-        <v>69</v>
+        <v>144</v>
       </c>
       <c r="E55" t="s">
         <v>25</v>
       </c>
       <c r="F55" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G55" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H55" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I55" t="s">
         <v>27</v>
       </c>
       <c r="J55" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K55" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L55" t="s">
         <v>28</v>
       </c>
       <c r="M55" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N55" t="s">
         <v>27</v>
       </c>
       <c r="O55" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P55" t="s">
         <v>27</v>
@@ -4388,19 +4424,19 @@
         <v>28</v>
       </c>
       <c r="R55" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S55" t="s">
         <v>28</v>
       </c>
       <c r="T55"/>
       <c r="U55" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B56" t="s">
         <v>49</v>
@@ -4409,16 +4445,16 @@
         <v>30</v>
       </c>
       <c r="D56" t="s">
-        <v>145</v>
+        <v>69</v>
       </c>
       <c r="E56" t="s">
         <v>25</v>
       </c>
       <c r="F56" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G56" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H56" t="s">
         <v>26</v>
@@ -4427,31 +4463,31 @@
         <v>27</v>
       </c>
       <c r="J56" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K56" t="s">
         <v>26</v>
       </c>
       <c r="L56" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M56" t="s">
         <v>27</v>
       </c>
       <c r="N56" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O56" t="s">
         <v>26</v>
       </c>
       <c r="P56" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q56" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="R56" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S56" t="s">
         <v>28</v>
@@ -4463,7 +4499,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B57" t="s">
         <v>49</v>
@@ -4490,25 +4526,25 @@
         <v>27</v>
       </c>
       <c r="J57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K57" t="s">
         <v>26</v>
       </c>
       <c r="L57" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M57" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N57" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O57" t="s">
         <v>26</v>
       </c>
       <c r="P57" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q57" t="s">
         <v>26</v>
@@ -4526,10 +4562,10 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B58" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C58" t="s">
         <v>30</v>
@@ -4541,19 +4577,19 @@
         <v>25</v>
       </c>
       <c r="F58" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G58" t="s">
         <v>27</v>
       </c>
       <c r="H58" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J58" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K58" t="s">
         <v>26</v>
@@ -4562,19 +4598,19 @@
         <v>28</v>
       </c>
       <c r="M58" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N58" t="s">
         <v>27</v>
       </c>
       <c r="O58" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q58" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R58" t="s">
         <v>26</v>
@@ -4589,46 +4625,46 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B59" t="s">
-        <v>61</v>
+        <v>151</v>
       </c>
       <c r="C59" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="D59" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E59" t="s">
         <v>25</v>
       </c>
       <c r="F59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I59" t="s">
         <v>28</v>
       </c>
       <c r="J59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L59" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N59" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O59" t="s">
         <v>27</v>
@@ -4637,106 +4673,108 @@
         <v>28</v>
       </c>
       <c r="Q59" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R59" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S59" t="s">
         <v>28</v>
       </c>
       <c r="T59"/>
       <c r="U59" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B60" t="s">
-        <v>61</v>
+        <v>151</v>
       </c>
       <c r="C60" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="D60" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E60" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F60" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G60" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H60" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I60" t="s">
         <v>28</v>
       </c>
       <c r="J60" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K60" t="s">
         <v>28</v>
       </c>
       <c r="L60" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M60" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N60" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O60" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P60" t="s">
         <v>28</v>
       </c>
       <c r="Q60" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R60" t="s">
         <v>28</v>
       </c>
       <c r="S60" t="s">
-        <v>27</v>
-      </c>
-      <c r="T60"/>
+        <v>28</v>
+      </c>
+      <c r="T60" t="s">
+        <v>155</v>
+      </c>
       <c r="U60" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B61" t="s">
-        <v>61</v>
+        <v>151</v>
       </c>
       <c r="C61" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="D61" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E61" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F61" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G61" t="s">
         <v>27</v>
       </c>
       <c r="H61" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I61" t="s">
         <v>28</v>
@@ -4748,13 +4786,13 @@
         <v>26</v>
       </c>
       <c r="L61" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M61" t="s">
         <v>27</v>
       </c>
       <c r="N61" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O61" t="s">
         <v>27</v>
@@ -4763,157 +4801,157 @@
         <v>28</v>
       </c>
       <c r="Q61" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="R61" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S61" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="T61"/>
       <c r="U61" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B62" t="s">
-        <v>71</v>
+        <v>151</v>
       </c>
       <c r="C62" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="D62" t="s">
-        <v>25</v>
+        <v>159</v>
       </c>
       <c r="E62" t="s">
         <v>25</v>
       </c>
       <c r="F62" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G62" t="s">
         <v>27</v>
       </c>
       <c r="H62" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I62" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J62" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K62" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L62" t="s">
         <v>28</v>
       </c>
       <c r="M62" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N62" t="s">
         <v>27</v>
       </c>
       <c r="O62" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P62" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q62" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R62" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S62" t="s">
         <v>28</v>
       </c>
       <c r="T62"/>
       <c r="U62" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B63" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C63" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="D63" t="s">
-        <v>35</v>
+        <v>161</v>
       </c>
       <c r="E63" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F63" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G63" t="s">
         <v>27</v>
       </c>
       <c r="H63" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I63" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J63" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K63" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L63" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M63" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N63" t="s">
         <v>27</v>
       </c>
       <c r="O63" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P63" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q63" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="R63" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S63" t="s">
         <v>28</v>
       </c>
       <c r="T63"/>
       <c r="U63" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B64" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C64" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="D64" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="E64" t="s">
         <v>25</v>
@@ -4922,37 +4960,37 @@
         <v>27</v>
       </c>
       <c r="G64" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H64" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I64" t="s">
         <v>28</v>
       </c>
       <c r="J64" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K64" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L64" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M64" t="s">
         <v>27</v>
       </c>
       <c r="N64" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O64" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P64" t="s">
         <v>28</v>
       </c>
       <c r="Q64" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R64" t="s">
         <v>28</v>
@@ -4962,84 +5000,84 @@
       </c>
       <c r="T64"/>
       <c r="U64" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C65" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="D65" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
       <c r="E65" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F65" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G65" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H65" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I65" t="s">
         <v>28</v>
       </c>
       <c r="J65" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K65" t="s">
         <v>28</v>
       </c>
       <c r="L65" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M65" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N65" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O65" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P65" t="s">
         <v>28</v>
       </c>
       <c r="Q65" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R65" t="s">
         <v>28</v>
       </c>
       <c r="S65" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T65"/>
       <c r="U65" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B66" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="C66" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="D66" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="E66" t="s">
         <v>25</v>
@@ -5051,19 +5089,19 @@
         <v>27</v>
       </c>
       <c r="H66" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I66" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J66" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K66" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L66" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M66" t="s">
         <v>27</v>
@@ -5072,37 +5110,37 @@
         <v>28</v>
       </c>
       <c r="O66" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P66" t="s">
         <v>28</v>
       </c>
       <c r="Q66" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R66" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S66" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T66"/>
       <c r="U66" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B67" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C67" t="s">
         <v>46</v>
       </c>
       <c r="D67" t="s">
-        <v>164</v>
+        <v>25</v>
       </c>
       <c r="E67" t="s">
         <v>25</v>
@@ -5117,16 +5155,16 @@
         <v>27</v>
       </c>
       <c r="I67" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J67" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K67" t="s">
         <v>27</v>
       </c>
       <c r="L67" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M67" t="s">
         <v>27</v>
@@ -5138,34 +5176,34 @@
         <v>27</v>
       </c>
       <c r="P67" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q67" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R67" t="s">
         <v>27</v>
       </c>
       <c r="S67" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="T67"/>
       <c r="U67" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B68" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C68" t="s">
         <v>46</v>
       </c>
       <c r="D68" t="s">
-        <v>166</v>
+        <v>35</v>
       </c>
       <c r="E68" t="s">
         <v>27</v>
@@ -5177,22 +5215,22 @@
         <v>27</v>
       </c>
       <c r="H68" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I68" t="s">
         <v>27</v>
       </c>
       <c r="J68" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K68" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L68" t="s">
         <v>27</v>
       </c>
       <c r="M68" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N68" t="s">
         <v>27</v>
@@ -5207,28 +5245,28 @@
         <v>27</v>
       </c>
       <c r="R68" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S68" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="T68"/>
       <c r="U68" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B69" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C69" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D69" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E69" t="s">
         <v>25</v>
@@ -5249,7 +5287,7 @@
         <v>28</v>
       </c>
       <c r="K69" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L69" t="s">
         <v>28</v>
@@ -5277,84 +5315,84 @@
       </c>
       <c r="T69"/>
       <c r="U69" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B70" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C70" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D70" t="s">
-        <v>170</v>
+        <v>116</v>
       </c>
       <c r="E70" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F70" t="s">
         <v>26</v>
       </c>
       <c r="G70" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H70" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I70" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J70" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K70" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L70" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M70" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N70" t="s">
         <v>28</v>
       </c>
       <c r="O70" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P70" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q70" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R70" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S70" t="s">
         <v>28</v>
       </c>
       <c r="T70"/>
       <c r="U70" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B71" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C71" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D71" t="s">
-        <v>52</v>
+        <v>174</v>
       </c>
       <c r="E71" t="s">
         <v>25</v>
@@ -5363,19 +5401,19 @@
         <v>27</v>
       </c>
       <c r="G71" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H71" t="s">
         <v>26</v>
       </c>
       <c r="I71" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J71" t="s">
         <v>28</v>
       </c>
       <c r="K71" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L71" t="s">
         <v>28</v>
@@ -5387,7 +5425,7 @@
         <v>28</v>
       </c>
       <c r="O71" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P71" t="s">
         <v>28</v>
@@ -5403,21 +5441,21 @@
       </c>
       <c r="T71"/>
       <c r="U71" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B72" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C72" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D72" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E72" t="s">
         <v>25</v>
@@ -5429,121 +5467,121 @@
         <v>27</v>
       </c>
       <c r="H72" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I72" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J72" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K72" t="s">
         <v>27</v>
       </c>
       <c r="L72" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M72" t="s">
         <v>27</v>
       </c>
       <c r="N72" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O72" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P72" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q72" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R72" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S72" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T72"/>
       <c r="U72" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B73" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C73" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D73" t="s">
-        <v>106</v>
+        <v>178</v>
       </c>
       <c r="E73" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F73" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G73" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H73" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I73" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J73" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K73" t="s">
         <v>26</v>
       </c>
       <c r="L73" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M73" t="s">
         <v>27</v>
       </c>
       <c r="N73" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O73" t="s">
         <v>27</v>
       </c>
       <c r="P73" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q73" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R73" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S73" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T73"/>
       <c r="U73" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B74" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C74" t="s">
         <v>23</v>
       </c>
       <c r="D74" t="s">
-        <v>88</v>
+        <v>180</v>
       </c>
       <c r="E74" t="s">
         <v>25</v>
@@ -5552,67 +5590,67 @@
         <v>27</v>
       </c>
       <c r="G74" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H74" t="s">
         <v>26</v>
       </c>
       <c r="I74" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J74" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K74" t="s">
         <v>26</v>
       </c>
       <c r="L74" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M74" t="s">
         <v>27</v>
       </c>
       <c r="N74" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O74" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P74" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q74" t="s">
         <v>28</v>
       </c>
       <c r="R74" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S74" t="s">
         <v>28</v>
       </c>
       <c r="T74"/>
       <c r="U74" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B75" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C75" t="s">
         <v>23</v>
       </c>
       <c r="D75" t="s">
-        <v>83</v>
+        <v>182</v>
       </c>
       <c r="E75" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F75" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G75" t="s">
         <v>27</v>
@@ -5627,7 +5665,7 @@
         <v>27</v>
       </c>
       <c r="K75" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L75" t="s">
         <v>27</v>
@@ -5636,10 +5674,10 @@
         <v>27</v>
       </c>
       <c r="N75" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O75" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P75" t="s">
         <v>27</v>
@@ -5655,21 +5693,21 @@
       </c>
       <c r="T75"/>
       <c r="U75" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B76" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C76" t="s">
         <v>23</v>
       </c>
       <c r="D76" t="s">
-        <v>178</v>
+        <v>52</v>
       </c>
       <c r="E76" t="s">
         <v>25</v>
@@ -5690,7 +5728,7 @@
         <v>28</v>
       </c>
       <c r="K76" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L76" t="s">
         <v>28</v>
@@ -5702,7 +5740,7 @@
         <v>28</v>
       </c>
       <c r="O76" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P76" t="s">
         <v>28</v>
@@ -5711,28 +5749,28 @@
         <v>28</v>
       </c>
       <c r="R76" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S76" t="s">
         <v>28</v>
       </c>
       <c r="T76"/>
       <c r="U76" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B77" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="C77" t="s">
         <v>23</v>
       </c>
       <c r="D77" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E77" t="s">
         <v>25</v>
@@ -5741,13 +5779,13 @@
         <v>27</v>
       </c>
       <c r="G77" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H77" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I77" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J77" t="s">
         <v>28</v>
@@ -5765,7 +5803,7 @@
         <v>28</v>
       </c>
       <c r="O77" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P77" t="s">
         <v>28</v>
@@ -5774,49 +5812,49 @@
         <v>28</v>
       </c>
       <c r="R77" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S77" t="s">
         <v>28</v>
       </c>
       <c r="T77"/>
       <c r="U77" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B78" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="C78" t="s">
         <v>23</v>
       </c>
       <c r="D78" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="E78" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F78" t="s">
         <v>27</v>
       </c>
       <c r="G78" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H78" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I78" t="s">
         <v>28</v>
       </c>
       <c r="J78" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K78" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L78" t="s">
         <v>28</v>
@@ -5834,7 +5872,7 @@
         <v>28</v>
       </c>
       <c r="Q78" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R78" t="s">
         <v>27</v>
@@ -5844,60 +5882,60 @@
       </c>
       <c r="T78"/>
       <c r="U78" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B79" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="C79" t="s">
         <v>23</v>
       </c>
       <c r="D79" t="s">
-        <v>183</v>
+        <v>88</v>
       </c>
       <c r="E79" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F79" t="s">
         <v>27</v>
       </c>
       <c r="G79" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H79" t="s">
         <v>26</v>
       </c>
       <c r="I79" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J79" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K79" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L79" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M79" t="s">
         <v>27</v>
       </c>
       <c r="N79" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O79" t="s">
         <v>27</v>
       </c>
       <c r="P79" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q79" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R79" t="s">
         <v>27</v>
@@ -5907,21 +5945,21 @@
       </c>
       <c r="T79"/>
       <c r="U79" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B80" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="C80" t="s">
         <v>23</v>
       </c>
       <c r="D80" t="s">
-        <v>185</v>
+        <v>83</v>
       </c>
       <c r="E80" t="s">
         <v>25</v>
@@ -5930,37 +5968,37 @@
         <v>27</v>
       </c>
       <c r="G80" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H80" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I80" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J80" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K80" t="s">
         <v>27</v>
       </c>
       <c r="L80" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M80" t="s">
         <v>27</v>
       </c>
       <c r="N80" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O80" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P80" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q80" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R80" t="s">
         <v>27</v>
@@ -5970,21 +6008,21 @@
       </c>
       <c r="T80"/>
       <c r="U80" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B81" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C81" t="s">
         <v>23</v>
       </c>
       <c r="D81" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E81" t="s">
         <v>25</v>
@@ -5993,19 +6031,19 @@
         <v>27</v>
       </c>
       <c r="G81" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H81" t="s">
         <v>26</v>
       </c>
       <c r="I81" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J81" t="s">
         <v>28</v>
       </c>
       <c r="K81" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L81" t="s">
         <v>28</v>
@@ -6014,7 +6052,7 @@
         <v>27</v>
       </c>
       <c r="N81" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O81" t="s">
         <v>26</v>
@@ -6023,103 +6061,103 @@
         <v>28</v>
       </c>
       <c r="Q81" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R81" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="S81" t="s">
         <v>28</v>
       </c>
       <c r="T81"/>
       <c r="U81" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B82" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="C82" t="s">
         <v>23</v>
       </c>
       <c r="D82" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E82" t="s">
         <v>25</v>
       </c>
       <c r="F82" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G82" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H82" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I82" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J82" t="s">
         <v>28</v>
       </c>
       <c r="K82" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L82" t="s">
         <v>28</v>
       </c>
       <c r="M82" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N82" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O82" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P82" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q82" t="s">
         <v>28</v>
       </c>
       <c r="R82" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="S82" t="s">
         <v>28</v>
       </c>
       <c r="T82"/>
       <c r="U82" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B83" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="C83" t="s">
         <v>23</v>
       </c>
       <c r="D83" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="E83" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F83" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G83" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H83" t="s">
         <v>26</v>
@@ -6128,10 +6166,10 @@
         <v>28</v>
       </c>
       <c r="J83" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K83" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L83" t="s">
         <v>28</v>
@@ -6143,46 +6181,46 @@
         <v>28</v>
       </c>
       <c r="O83" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P83" t="s">
         <v>28</v>
       </c>
       <c r="Q83" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R83" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S83" t="s">
         <v>28</v>
       </c>
       <c r="T83"/>
       <c r="U83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B84" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="C84" t="s">
         <v>23</v>
       </c>
       <c r="D84" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E84" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F84" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G84" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H84" t="s">
         <v>26</v>
@@ -6194,35 +6232,350 @@
         <v>28</v>
       </c>
       <c r="K84" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L84" t="s">
         <v>28</v>
       </c>
       <c r="M84" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N84" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="O84" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P84" t="s">
         <v>28</v>
       </c>
       <c r="Q84" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R84" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S84" t="s">
         <v>28</v>
       </c>
       <c r="T84"/>
       <c r="U84" t="s">
-        <v>193</v>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>123</v>
+      </c>
+      <c r="B85" t="s">
+        <v>113</v>
+      </c>
+      <c r="C85" t="s">
+        <v>23</v>
+      </c>
+      <c r="D85" t="s">
+        <v>197</v>
+      </c>
+      <c r="E85" t="s">
+        <v>25</v>
+      </c>
+      <c r="F85" t="s">
+        <v>27</v>
+      </c>
+      <c r="G85" t="s">
+        <v>28</v>
+      </c>
+      <c r="H85" t="s">
+        <v>27</v>
+      </c>
+      <c r="I85" t="s">
+        <v>28</v>
+      </c>
+      <c r="J85" t="s">
+        <v>28</v>
+      </c>
+      <c r="K85" t="s">
+        <v>27</v>
+      </c>
+      <c r="L85" t="s">
+        <v>28</v>
+      </c>
+      <c r="M85" t="s">
+        <v>27</v>
+      </c>
+      <c r="N85" t="s">
+        <v>28</v>
+      </c>
+      <c r="O85" t="s">
+        <v>27</v>
+      </c>
+      <c r="P85" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>28</v>
+      </c>
+      <c r="R85" t="s">
+        <v>27</v>
+      </c>
+      <c r="S85" t="s">
+        <v>28</v>
+      </c>
+      <c r="T85"/>
+      <c r="U85" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>123</v>
+      </c>
+      <c r="B86" t="s">
+        <v>113</v>
+      </c>
+      <c r="C86" t="s">
+        <v>23</v>
+      </c>
+      <c r="D86" t="s">
+        <v>199</v>
+      </c>
+      <c r="E86" t="s">
+        <v>25</v>
+      </c>
+      <c r="F86" t="s">
+        <v>27</v>
+      </c>
+      <c r="G86" t="s">
+        <v>25</v>
+      </c>
+      <c r="H86" t="s">
+        <v>26</v>
+      </c>
+      <c r="I86" t="s">
+        <v>27</v>
+      </c>
+      <c r="J86" t="s">
+        <v>28</v>
+      </c>
+      <c r="K86" t="s">
+        <v>28</v>
+      </c>
+      <c r="L86" t="s">
+        <v>28</v>
+      </c>
+      <c r="M86" t="s">
+        <v>27</v>
+      </c>
+      <c r="N86" t="s">
+        <v>27</v>
+      </c>
+      <c r="O86" t="s">
+        <v>26</v>
+      </c>
+      <c r="P86" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>27</v>
+      </c>
+      <c r="R86" t="s">
+        <v>25</v>
+      </c>
+      <c r="S86" t="s">
+        <v>28</v>
+      </c>
+      <c r="T86"/>
+      <c r="U86" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>123</v>
+      </c>
+      <c r="B87" t="s">
+        <v>103</v>
+      </c>
+      <c r="C87" t="s">
+        <v>23</v>
+      </c>
+      <c r="D87" t="s">
+        <v>201</v>
+      </c>
+      <c r="E87" t="s">
+        <v>25</v>
+      </c>
+      <c r="F87" t="s">
+        <v>28</v>
+      </c>
+      <c r="G87" t="s">
+        <v>27</v>
+      </c>
+      <c r="H87" t="s">
+        <v>26</v>
+      </c>
+      <c r="I87" t="s">
+        <v>27</v>
+      </c>
+      <c r="J87" t="s">
+        <v>28</v>
+      </c>
+      <c r="K87" t="s">
+        <v>28</v>
+      </c>
+      <c r="L87" t="s">
+        <v>28</v>
+      </c>
+      <c r="M87" t="s">
+        <v>28</v>
+      </c>
+      <c r="N87" t="s">
+        <v>27</v>
+      </c>
+      <c r="O87" t="s">
+        <v>26</v>
+      </c>
+      <c r="P87" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>28</v>
+      </c>
+      <c r="R87" t="s">
+        <v>25</v>
+      </c>
+      <c r="S87" t="s">
+        <v>28</v>
+      </c>
+      <c r="T87"/>
+      <c r="U87" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>123</v>
+      </c>
+      <c r="B88" t="s">
+        <v>103</v>
+      </c>
+      <c r="C88" t="s">
+        <v>23</v>
+      </c>
+      <c r="D88" t="s">
+        <v>149</v>
+      </c>
+      <c r="E88" t="s">
+        <v>25</v>
+      </c>
+      <c r="F88" t="s">
+        <v>26</v>
+      </c>
+      <c r="G88" t="s">
+        <v>28</v>
+      </c>
+      <c r="H88" t="s">
+        <v>26</v>
+      </c>
+      <c r="I88" t="s">
+        <v>28</v>
+      </c>
+      <c r="J88" t="s">
+        <v>28</v>
+      </c>
+      <c r="K88" t="s">
+        <v>26</v>
+      </c>
+      <c r="L88" t="s">
+        <v>28</v>
+      </c>
+      <c r="M88" t="s">
+        <v>27</v>
+      </c>
+      <c r="N88" t="s">
+        <v>28</v>
+      </c>
+      <c r="O88" t="s">
+        <v>26</v>
+      </c>
+      <c r="P88" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>28</v>
+      </c>
+      <c r="R88" t="s">
+        <v>26</v>
+      </c>
+      <c r="S88" t="s">
+        <v>28</v>
+      </c>
+      <c r="T88"/>
+      <c r="U88" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>123</v>
+      </c>
+      <c r="B89" t="s">
+        <v>103</v>
+      </c>
+      <c r="C89" t="s">
+        <v>23</v>
+      </c>
+      <c r="D89" t="s">
+        <v>204</v>
+      </c>
+      <c r="E89" t="s">
+        <v>25</v>
+      </c>
+      <c r="F89" t="s">
+        <v>26</v>
+      </c>
+      <c r="G89" t="s">
+        <v>27</v>
+      </c>
+      <c r="H89" t="s">
+        <v>26</v>
+      </c>
+      <c r="I89" t="s">
+        <v>27</v>
+      </c>
+      <c r="J89" t="s">
+        <v>28</v>
+      </c>
+      <c r="K89" t="s">
+        <v>26</v>
+      </c>
+      <c r="L89" t="s">
+        <v>28</v>
+      </c>
+      <c r="M89" t="s">
+        <v>28</v>
+      </c>
+      <c r="N89" t="s">
+        <v>28</v>
+      </c>
+      <c r="O89" t="s">
+        <v>26</v>
+      </c>
+      <c r="P89" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>28</v>
+      </c>
+      <c r="R89" t="s">
+        <v>28</v>
+      </c>
+      <c r="S89" t="s">
+        <v>28</v>
+      </c>
+      <c r="T89"/>
+      <c r="U89" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>